<commit_message>
Maybe really working, added RSSI test
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.5.xlsx
+++ b/ProductionTests/Sthv2.1.5.xlsx
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>20191002</t>
+          <t>20191003</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>0.29144731163978577</t>
+          <t>0.34332799911499023</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>0.07782012969255447</t>
+          <t>0.057728882879018784</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>

</xml_diff>

<commit_message>
Production Tests ready, automatic programming will come Standby after last successful test bugs... better EEPROM internal verfication test for STU too
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.5.xlsx
+++ b/ProductionTests/Sthv2.1.5.xlsx
@@ -1367,7 +1367,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>20191008</t>
+          <t>20191009</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>0.003052281215786934</t>
+          <t>0.0030518043786287308</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>-99.65972137451172</t>
+          <t>-99.62920379638672</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>0.057728882879018784</t>
+          <t>0.07954223453998566</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>

</xml_diff>

<commit_message>
debug access granted (Manufacturing flash) working :)
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.5.xlsx
+++ b/ProductionTests/Sthv2.1.5.xlsx
@@ -1367,7 +1367,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>20191009</t>
+          <t>20191021</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>

</xml_diff>